<commit_message>
checking in code and figures
</commit_message>
<xml_diff>
--- a/expression_data/abl1-construct/abl1-constructs-fulldata.xlsx
+++ b/expression_data/abl1-construct/abl1-constructs-fulldata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14520"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Abl1_constructs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -558,16 +558,16 @@
     <t>Construct</t>
   </si>
   <si>
-    <t>Concentration</t>
-  </si>
-  <si>
     <t>N terminus</t>
   </si>
   <si>
     <t>C terminus</t>
   </si>
   <si>
-    <t>scaled up yield</t>
+    <t xml:space="preserve">Concentration (ug/ml) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yield per ml culture (ug/ml) </t>
   </si>
 </sst>
 </file>
@@ -931,7 +931,7 @@
   <dimension ref="A1:K97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -950,13 +950,13 @@
         <v>178</v>
       </c>
       <c r="C1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" t="s">
         <v>180</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>181</v>
-      </c>
-      <c r="E1" t="s">
-        <v>179</v>
       </c>
       <c r="F1" t="s">
         <v>182</v>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <f>E2*80/900</f>
+        <f t="shared" ref="F2:F33" si="0">E2*80/900</f>
         <v>0</v>
       </c>
     </row>
@@ -1000,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f>E3*80/900</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1021,11 +1021,11 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f>E4*80/900</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1042,11 +1042,11 @@
         <v>7.50883079783633</v>
       </c>
       <c r="F5">
-        <f>E5*80/900</f>
+        <f t="shared" si="0"/>
         <v>0.66745162647434053</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -1063,11 +1063,11 @@
         <v>4.9041031250759399</v>
       </c>
       <c r="F6">
-        <f>E6*80/900</f>
+        <f t="shared" si="0"/>
         <v>0.43592027778452802</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>17.704699400795199</v>
       </c>
       <c r="F7">
-        <f>E7*80/900</f>
+        <f t="shared" si="0"/>
         <v>1.5737510578484621</v>
       </c>
     </row>
@@ -1105,7 +1105,7 @@
         <v>29.9535274392133</v>
       </c>
       <c r="F8">
-        <f>E8*80/900</f>
+        <f t="shared" si="0"/>
         <v>2.6625357723745156</v>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
         <v>22.2816804204374</v>
       </c>
       <c r="F9">
-        <f>E9*80/900</f>
+        <f t="shared" si="0"/>
         <v>1.9805938151499911</v>
       </c>
     </row>
@@ -1147,7 +1147,7 @@
         <v>22.924422118282902</v>
       </c>
       <c r="F10">
-        <f>E10*80/900</f>
+        <f t="shared" si="0"/>
         <v>2.0377264105140358</v>
       </c>
     </row>
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <f>E11*80/900</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <f>E12*80/900</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <f>E13*80/900</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1231,11 +1231,11 @@
         <v>11.4338889921519</v>
       </c>
       <c r="F14">
-        <f>E14*80/900</f>
+        <f t="shared" si="0"/>
         <v>1.01634568819128</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>6</v>
       </c>
       <c r="F15">
-        <f>E15*80/900</f>
+        <f t="shared" si="0"/>
         <v>0.53333333333333333</v>
       </c>
     </row>
@@ -1273,7 +1273,7 @@
         <v>10.6160531632318</v>
       </c>
       <c r="F16">
-        <f>E16*80/900</f>
+        <f t="shared" si="0"/>
         <v>0.94364917006504889</v>
       </c>
     </row>
@@ -1294,7 +1294,7 @@
         <v>19.492927648887001</v>
       </c>
       <c r="F17">
-        <f>E17*80/900</f>
+        <f t="shared" si="0"/>
         <v>1.7327046799010668</v>
       </c>
     </row>
@@ -1315,7 +1315,7 @@
         <v>14</v>
       </c>
       <c r="F18">
-        <f>E18*80/900</f>
+        <f t="shared" si="0"/>
         <v>1.2444444444444445</v>
       </c>
     </row>
@@ -1336,7 +1336,7 @@
         <v>14</v>
       </c>
       <c r="F19">
-        <f>E19*80/900</f>
+        <f t="shared" si="0"/>
         <v>1.2444444444444445</v>
       </c>
     </row>
@@ -1357,7 +1357,7 @@
         <v>9.2902432118685496</v>
       </c>
       <c r="F20">
-        <f>E20*80/900</f>
+        <f t="shared" si="0"/>
         <v>0.82579939661053769</v>
       </c>
     </row>
@@ -1378,11 +1378,11 @@
         <v>22.340835929906099</v>
       </c>
       <c r="F21">
-        <f>E21*80/900</f>
+        <f t="shared" si="0"/>
         <v>1.9858520826583197</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" ht="15">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>39</v>
       </c>
       <c r="F22">
-        <f>E22*80/900</f>
+        <f t="shared" si="0"/>
         <v>3.4666666666666668</v>
       </c>
       <c r="I22" t="s">
@@ -1431,7 +1431,7 @@
         <v>23.295327915246801</v>
       </c>
       <c r="F23">
-        <f>E23*80/900</f>
+        <f t="shared" si="0"/>
         <v>2.0706958146886048</v>
       </c>
       <c r="I23" t="s">
@@ -1463,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <f>E24*80/900</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I24" t="s">
@@ -1495,7 +1495,7 @@
         <v>42</v>
       </c>
       <c r="F25">
-        <f>E25*80/900</f>
+        <f t="shared" si="0"/>
         <v>3.7333333333333334</v>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
         <v>42</v>
       </c>
       <c r="F26">
-        <f>E26*80/900</f>
+        <f t="shared" si="0"/>
         <v>3.7333333333333334</v>
       </c>
     </row>
@@ -1537,7 +1537,7 @@
         <v>38.404274217294898</v>
       </c>
       <c r="F27">
-        <f>E27*80/900</f>
+        <f t="shared" si="0"/>
         <v>3.4137132637595466</v>
       </c>
     </row>
@@ -1558,11 +1558,11 @@
         <v>46.575212477776198</v>
       </c>
       <c r="F28">
-        <f>E28*80/900</f>
+        <f t="shared" si="0"/>
         <v>4.14001888691344</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" ht="15">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>40</v>
       </c>
       <c r="F29">
-        <f>E29*80/900</f>
+        <f t="shared" si="0"/>
         <v>3.5555555555555554</v>
       </c>
     </row>
@@ -1600,7 +1600,7 @@
         <v>22.4975436748677</v>
       </c>
       <c r="F30">
-        <f>E30*80/900</f>
+        <f t="shared" si="0"/>
         <v>1.9997816599882401</v>
       </c>
     </row>
@@ -1621,7 +1621,7 @@
         <v>34.3100192563899</v>
       </c>
       <c r="F31">
-        <f>E31*80/900</f>
+        <f t="shared" si="0"/>
         <v>3.0497794894568799</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
         <v>30</v>
       </c>
       <c r="F32">
-        <f>E32*80/900</f>
+        <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
         <v>35</v>
       </c>
       <c r="F33">
-        <f>E33*80/900</f>
+        <f t="shared" si="0"/>
         <v>3.1111111111111112</v>
       </c>
     </row>
@@ -1684,7 +1684,7 @@
         <v>30.7539399291881</v>
       </c>
       <c r="F34">
-        <f>E34*80/900</f>
+        <f t="shared" ref="F34:F65" si="1">E34*80/900</f>
         <v>2.7336835492611646</v>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <f>E35*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1726,7 +1726,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <f>E36*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <f>E37*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
         <v>8.4436318465309004</v>
       </c>
       <c r="F38">
-        <f>E38*80/900</f>
+        <f t="shared" si="1"/>
         <v>0.75054505302496888</v>
       </c>
     </row>
@@ -1789,7 +1789,7 @@
         <v>21.7497992180046</v>
       </c>
       <c r="F39">
-        <f>E39*80/900</f>
+        <f t="shared" si="1"/>
         <v>1.9333154860448534</v>
       </c>
     </row>
@@ -1810,7 +1810,7 @@
         <v>36.324032105220297</v>
       </c>
       <c r="F40">
-        <f>E40*80/900</f>
+        <f t="shared" si="1"/>
         <v>3.2288028537973594</v>
       </c>
     </row>
@@ -1831,7 +1831,7 @@
         <v>46.185433077641797</v>
       </c>
       <c r="F41">
-        <f>E41*80/900</f>
+        <f t="shared" si="1"/>
         <v>4.1053718291237153</v>
       </c>
     </row>
@@ -1852,7 +1852,7 @@
         <v>48.638545858003297</v>
       </c>
       <c r="F42">
-        <f>E42*80/900</f>
+        <f t="shared" si="1"/>
         <v>4.3234262984891814</v>
       </c>
     </row>
@@ -1873,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <f>E43*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1894,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <f>E44*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <f>E45*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1936,7 +1936,7 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <f>E46*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <f>E47*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <f>E48*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1999,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <f>E49*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2020,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <f>E50*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2041,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <f>E51*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="F52">
-        <f>E52*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2083,7 +2083,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <f>E53*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2104,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <f>E54*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2125,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <f>E55*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2146,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <f>E56*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <f>E57*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2188,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <f>E58*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <f>E59*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2230,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <f>E60*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2251,7 +2251,7 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <f>E61*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2272,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <f>E62*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2293,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <f>E63*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <f>E64*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2335,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <f>E65*80/900</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2356,7 +2356,7 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <f>E66*80/900</f>
+        <f t="shared" ref="F66:F97" si="2">E66*80/900</f>
         <v>0</v>
       </c>
     </row>
@@ -2377,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <f>E67*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2398,7 +2398,7 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <f>E68*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <f>E69*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2440,7 +2440,7 @@
         <v>2007</v>
       </c>
       <c r="F70">
-        <f>E70*80/900</f>
+        <f t="shared" si="2"/>
         <v>178.4</v>
       </c>
     </row>
@@ -2461,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="F71">
-        <f>E71*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2482,7 +2482,7 @@
         <v>0</v>
       </c>
       <c r="F72">
-        <f>E72*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2503,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="F73">
-        <f>E73*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2524,7 +2524,7 @@
         <v>0</v>
       </c>
       <c r="F74">
-        <f>E74*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2545,7 +2545,7 @@
         <v>0</v>
       </c>
       <c r="F75">
-        <f>E75*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2566,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="F76">
-        <f>E76*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2587,7 +2587,7 @@
         <v>0</v>
       </c>
       <c r="F77">
-        <f>E77*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2608,7 +2608,7 @@
         <v>3</v>
       </c>
       <c r="F78">
-        <f>E78*80/900</f>
+        <f t="shared" si="2"/>
         <v>0.26666666666666666</v>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
         <v>0</v>
       </c>
       <c r="F79">
-        <f>E79*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2650,7 +2650,7 @@
         <v>0</v>
       </c>
       <c r="F80">
-        <f>E80*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2671,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="F81">
-        <f>E81*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2692,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="F82">
-        <f>E82*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2713,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="F83">
-        <f>E83*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2734,7 +2734,7 @@
         <v>0</v>
       </c>
       <c r="F84">
-        <f>E84*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2755,7 +2755,7 @@
         <v>0</v>
       </c>
       <c r="F85">
-        <f>E85*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2776,7 +2776,7 @@
         <v>0</v>
       </c>
       <c r="F86">
-        <f>E86*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2797,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="F87">
-        <f>E87*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2818,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="F88">
-        <f>E88*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2839,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="F89">
-        <f>E89*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2860,7 +2860,7 @@
         <v>0</v>
       </c>
       <c r="F90">
-        <f>E90*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2881,7 +2881,7 @@
         <v>0</v>
       </c>
       <c r="F91">
-        <f>E91*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2902,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="F92">
-        <f>E92*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2923,7 +2923,7 @@
         <v>0</v>
       </c>
       <c r="F93">
-        <f>E93*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2944,7 +2944,7 @@
         <v>0</v>
       </c>
       <c r="F94">
-        <f>E94*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2965,7 +2965,7 @@
         <v>0</v>
       </c>
       <c r="F95">
-        <f>E95*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2986,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="F96">
-        <f>E96*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3007,7 +3007,7 @@
         <v>0</v>
       </c>
       <c r="F97">
-        <f>E97*80/900</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>